<commit_message>
Hub airport selection for COP29
</commit_message>
<xml_diff>
--- a/output/non_direct_flights_statistics.xlsx
+++ b/output/non_direct_flights_statistics.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ls2823_ic_ac_uk/Documents/0_Sustainable Transport/COP_flight_analysis/output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_C1BF870BA031921FD2FE31D2F8F2D3C2F4D370B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9D24A76-FF20-4B46-AAA2-235D5F67F3FB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>assumed_load_factor</t>
   </si>
@@ -47,28 +41,13 @@
   </si>
   <si>
     <t>sulphates_kg</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,33 +99,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,7 +154,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -218,7 +188,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -253,10 +222,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,303 +397,272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>178</v>
       </c>
       <c r="B2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="D2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="E2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="F2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="G2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="H2">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="I2">
-        <v>166</v>
-      </c>
-      <c r="J2">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>0.6643780106867584</v>
       </c>
       <c r="B3">
-        <v>0.68627902306180855</v>
+        <v>21371.08718062585</v>
       </c>
       <c r="C3">
-        <v>39386.542820703376</v>
+        <v>67511.26440359706</v>
       </c>
       <c r="D3">
-        <v>124422.088770602</v>
+        <v>297.9250240809672</v>
       </c>
       <c r="E3">
-        <v>812.36909321038138</v>
+        <v>3.830315180447156</v>
       </c>
       <c r="F3">
-        <v>3.8189911438758788</v>
+        <v>0.4274217436125169</v>
       </c>
       <c r="G3">
-        <v>0.78773085641406748</v>
+        <v>26286.43723216979</v>
       </c>
       <c r="H3">
-        <v>48445.44766946516</v>
+        <v>25.64530461675102</v>
       </c>
       <c r="I3">
-        <v>47.263851384844052</v>
-      </c>
-      <c r="J3">
-        <v>0.96456839560906238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
+        <v>0.5233735636071636</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>0.07104235951591743</v>
       </c>
       <c r="B4">
-        <v>7.4330439769259862E-2</v>
+        <v>29143.57529388768</v>
       </c>
       <c r="C4">
-        <v>44207.891315282868</v>
+        <v>92064.5543533912</v>
       </c>
       <c r="D4">
-        <v>139652.72866497861</v>
+        <v>420.2761367823823</v>
       </c>
       <c r="E4">
-        <v>987.22035735927091</v>
+        <v>11.78394463056079</v>
       </c>
       <c r="F4">
-        <v>4.0242870679632912</v>
+        <v>0.5828715058777537</v>
       </c>
       <c r="G4">
-        <v>0.88415782630565742</v>
+        <v>35846.59761148185</v>
       </c>
       <c r="H4">
-        <v>54375.706317797929</v>
+        <v>34.97229035266522</v>
       </c>
       <c r="I4">
-        <v>53.049469578339441</v>
-      </c>
-      <c r="J4">
-        <v>1.082642236292642</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
+        <v>0.713720211278882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>0.5245896810666667</v>
       </c>
       <c r="B5">
-        <v>0.60607934019999998</v>
+        <v>130.2398200270152</v>
       </c>
       <c r="C5">
-        <v>162.6064309985131</v>
+        <v>411.427591465341</v>
       </c>
       <c r="D5">
-        <v>513.67371552430279</v>
+        <v>1.97183087520901</v>
       </c>
       <c r="E5">
-        <v>2.461861365317489</v>
+        <v>0.0129935579494328</v>
       </c>
       <c r="F5">
-        <v>8.6314556960900117E-3</v>
+        <v>0.002604796400540304</v>
       </c>
       <c r="G5">
-        <v>3.252128619970263E-3</v>
+        <v>160.1949786332287</v>
       </c>
       <c r="H5">
-        <v>200.00591012817111</v>
+        <v>0.1562877840324182</v>
       </c>
       <c r="I5">
-        <v>0.19512771719821581</v>
-      </c>
-      <c r="J5">
-        <v>3.9821983101676678E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>0.25</v>
+        <v>0.003189546612906494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>0.6219998006290323</v>
       </c>
       <c r="B6">
-        <v>0.60695517739999993</v>
+        <v>2670.826547004206</v>
       </c>
       <c r="C6">
-        <v>5633.2952517758113</v>
+        <v>8437.141061986287</v>
       </c>
       <c r="D6">
-        <v>17795.57970035978</v>
+        <v>34.30270701481645</v>
       </c>
       <c r="E6">
-        <v>70.74213196412235</v>
+        <v>0.3651244385771767</v>
       </c>
       <c r="F6">
-        <v>0.65588944271033089</v>
+        <v>0.05341653094008411</v>
       </c>
       <c r="G6">
-        <v>0.1126659050355162</v>
+        <v>3285.116652815173</v>
       </c>
       <c r="H6">
-        <v>6928.9531596842462</v>
+        <v>3.204991856405047</v>
       </c>
       <c r="I6">
-        <v>6.7599543021309714</v>
-      </c>
-      <c r="J6">
-        <v>0.13795825106389739</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>0.5</v>
+        <v>0.06540799706949076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>0.6987738282666667</v>
       </c>
       <c r="B7">
-        <v>0.66146120083333337</v>
+        <v>7649.937557589101</v>
       </c>
       <c r="C7">
-        <v>12195.44139136002</v>
+        <v>24166.15274442397</v>
       </c>
       <c r="D7">
-        <v>38525.399355306297</v>
+        <v>86.03013237340585</v>
       </c>
       <c r="E7">
-        <v>187.3752970968242</v>
+        <v>0.811637069816892</v>
       </c>
       <c r="F7">
-        <v>1.154801533386608</v>
+        <v>0.152998751151782</v>
       </c>
       <c r="G7">
-        <v>0.24390882782720039</v>
+        <v>9409.423195834595</v>
       </c>
       <c r="H7">
-        <v>15000.392911372821</v>
+        <v>9.17992506910692</v>
       </c>
       <c r="I7">
-        <v>14.63452966963202</v>
-      </c>
-      <c r="J7">
-        <v>0.29866387080881679</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>0.75</v>
+        <v>0.1873454095736106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0.7073570327833333</v>
       </c>
       <c r="B8">
-        <v>0.75174210653333329</v>
+        <v>31964.284773864</v>
       </c>
       <c r="C8">
-        <v>65141.195456496927</v>
+        <v>100975.1756006364</v>
       </c>
       <c r="D8">
-        <v>205781.0364470738</v>
+        <v>420.0714217200809</v>
       </c>
       <c r="E8">
-        <v>1310.0052346494399</v>
+        <v>3.582394935444827</v>
       </c>
       <c r="F8">
-        <v>6.8465265181043424</v>
+        <v>0.6392856954772799</v>
       </c>
       <c r="G8">
-        <v>1.302823909129939</v>
+        <v>39316.07027185272</v>
       </c>
       <c r="H8">
-        <v>80123.670411491243</v>
+        <v>38.3571417286368</v>
       </c>
       <c r="I8">
-        <v>78.169434547796328</v>
-      </c>
-      <c r="J8">
-        <v>1.595294582608088</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>13</v>
+        <v>0.782798810788506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>0.8116680160999999</v>
       </c>
       <c r="B9">
-        <v>0.81318515250000001</v>
+        <v>112020.975968936</v>
       </c>
       <c r="C9">
-        <v>145152.18210084879</v>
+        <v>353874.2630858688</v>
       </c>
       <c r="D9">
-        <v>458535.74325658119</v>
+        <v>1589.736681983776</v>
       </c>
       <c r="E9">
-        <v>2871.4521899726351</v>
+        <v>76.16236322150311</v>
       </c>
       <c r="F9">
-        <v>18.037676425320591</v>
+        <v>2.24041951937872</v>
       </c>
       <c r="G9">
-        <v>2.903043642016975</v>
+        <v>137785.8004417912</v>
       </c>
       <c r="H9">
-        <v>178537.18398404401</v>
+        <v>134.4251711627232</v>
       </c>
       <c r="I9">
-        <v>174.1826185210185</v>
-      </c>
-      <c r="J9">
-        <v>3.5547473167554791</v>
+        <v>2.743370840055575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>